<commit_message>
login page added @10/05/2018
</commit_message>
<xml_diff>
--- a/zoom12/src/testsuit/zoom12user.xlsx
+++ b/zoom12/src/testsuit/zoom12user.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="11490" windowHeight="5595" activeTab="1"/>
+    <workbookView windowWidth="9645" windowHeight="6585" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102">
   <si>
     <t>Componet</t>
   </si>
@@ -203,70 +203,40 @@
     <t>21-50</t>
   </si>
   <si>
-    <t>NVIDIA Corporation2</t>
-  </si>
-  <si>
-    <t>Mr.Shani</t>
-  </si>
-  <si>
-    <t>zoomattest82@mailinator.com</t>
-  </si>
-  <si>
-    <t>company description2</t>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Skills</t>
+  </si>
+  <si>
+    <t>Industry you cater to</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>Automobiles</t>
+  </si>
+  <si>
+    <t>Mixed Reality (VR and AR)</t>
   </si>
   <si>
     <t>Automotive</t>
   </si>
   <si>
+    <t>UI/UX</t>
+  </si>
+  <si>
+    <t>BFSI</t>
+  </si>
+  <si>
     <t>Social &amp; Mobility</t>
   </si>
   <si>
+    <t>Banking</t>
+  </si>
+  <si>
     <t>Big Data &amp; Analytics</t>
-  </si>
-  <si>
-    <t>2000</t>
-  </si>
-  <si>
-    <t>Deployment</t>
-  </si>
-  <si>
-    <t>5000</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>800000</t>
-  </si>
-  <si>
-    <t>Mr shani</t>
-  </si>
-  <si>
-    <t>101-250</t>
-  </si>
-  <si>
-    <t>Currency</t>
-  </si>
-  <si>
-    <t>Skills</t>
-  </si>
-  <si>
-    <t>Industry you cater to</t>
-  </si>
-  <si>
-    <t>Automobiles</t>
-  </si>
-  <si>
-    <t>Mixed Reality (VR and AR)</t>
-  </si>
-  <si>
-    <t>UI/UX</t>
-  </si>
-  <si>
-    <t>BFSI</t>
-  </si>
-  <si>
-    <t>Banking</t>
   </si>
   <si>
     <t>CPG</t>
@@ -382,10 +352,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -437,7 +407,113 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -452,113 +528,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -585,187 +555,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -813,31 +783,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -859,6 +805,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -868,11 +823,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -891,153 +852,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1452,13 +1422,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:X4"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="34.1428571428571" style="3" customWidth="1"/>
     <col min="2" max="2" width="28.1428571428571" style="3" customWidth="1"/>
@@ -1629,140 +1599,59 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" ht="60" spans="1:24">
-      <c r="A3" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="14:14">
-      <c r="N4" s="3">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <dataValidations count="16">
-    <dataValidation type="textLength" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="please enter less than 512" prompt="aplha numberic all chars allowed" sqref="E2 E3 E4:E1048576">
+    <dataValidation type="textLength" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="please enter company name with in 512 chars" prompt="maxium 512 chars allowed" sqref="A2 A3:A1048576">
       <formula1>1</formula1>
       <formula2>512</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="select from dropdown only&#10;" sqref="G2 H2 G3 H3 G4:G1048576 H4:H1048576">
-      <formula1>Sheet4!$B$2:$B$14</formula1>
+    <dataValidation type="textLength" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="maximum allowed 50 chars in alphabet with dot, spaces, hyphen, aphostrophe" prompt="please enter atleat one char" sqref="B2 B3:B1048576">
+      <formula1>1</formula1>
+      <formula2>50</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="please enter valid web url" sqref="I2 I3 I4:I1048576"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2 O2 M3 O3 M4:M1048576 O4:O1048576">
-      <formula1>Sheet4!$A$2:$A$3</formula1>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="please enter valid email" sqref="C2 C3:C1048576"/>
+    <dataValidation type="textLength" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="space, dot commas, aphostropee, characters maximum 64 characters are allowed" sqref="D2 D3:D1048576">
+      <formula1>1</formula1>
+      <formula2>64</formula2>
     </dataValidation>
-    <dataValidation type="textLength" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="please enter company name with in 512 chars" prompt="maxium 512 chars allowed" sqref="A2:A1048576">
+    <dataValidation type="textLength" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="please enter less than 512" prompt="aplha numberic all chars allowed" sqref="E2 E3:E1048576">
       <formula1>1</formula1>
       <formula2>512</formula2>
     </dataValidation>
-    <dataValidation type="textLength" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="maximum allowed 50 chars in alphabet with dot, spaces, hyphen, aphostrophe" prompt="please enter atleat one char" sqref="B2:B1048576">
-      <formula1>1</formula1>
-      <formula2>50</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="please enter valid email" sqref="C2:C3 C4:C1048576"/>
-    <dataValidation type="textLength" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="space, dot commas, aphostropee, characters maximum 64 characters are allowed" sqref="D2:D3 D4:D1048576">
-      <formula1>1</formula1>
-      <formula2>64</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="please select" sqref="F2:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="please select" sqref="F2 F3:F1048576">
       <formula1>Sheet4!$C$2:$C$36</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="select from dropdown only&#10;" sqref="G2 H2 G3:G1048576 H3:H1048576">
+      <formula1>Sheet4!$B$2:$B$14</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="please enter valid web url" sqref="I2 I3:I1048576"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2 K3:K1048576">
       <formula1>"Deployment,Alpha,Beta,Production,Other"</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="more than 512 chars" prompt="only 512 chars are allowed" sqref="P2:P1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2 O2 M3:M1048576 O3:O1048576">
+      <formula1>Sheet4!$A$2:$A$3</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="more than 512 chars" prompt="only 512 chars are allowed" sqref="P2 P3:P1048576">
       <formula1>0</formula1>
       <formula2>512</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="please enter prefix code " sqref="U2:U1048576"/>
-    <dataValidation type="whole" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="enter only numbers max 15 chars" prompt="only numbers allowed" sqref="V2:V1048576">
+    <dataValidation type="textLength" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="max chars 30 allowed only" prompt="please enter value , its mandatory" sqref="Q2:T2 Q3:T1048576">
+      <formula1>1</formula1>
+      <formula2>30</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="please enter prefix code " sqref="U2 U3:U1048576"/>
+    <dataValidation type="whole" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="enter only numbers max 15 chars" prompt="only numbers allowed" sqref="V2 V3:V1048576">
       <formula1>0</formula1>
       <formula2>15</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="only text with char, - ' allowed" sqref="W2:W1048576"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2:X1048576">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="only text with char, - ' allowed" sqref="W2 W3:W1048576"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2 X3:X1048576">
       <formula1>"0-10,11-20,21-50,51-100,101-250,251-500,500+"</formula1>
-    </dataValidation>
-    <dataValidation type="textLength" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="max chars 30 allowed only" prompt="please enter value , its mandatory" sqref="Q2:T1048576">
-      <formula1>1</formula1>
-      <formula2>30</formula2>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="zoomattest81@mailinator.com" tooltip="mailto:zoomattest81@mailinator.com"/>
-    <hyperlink ref="C3" r:id="rId1" display="zoomattest82@mailinator.com" tooltip="mailto:zoomattest81@mailinator.com"/>
     <hyperlink ref="I2" r:id="rId2" display="https://www.nvdia.com"/>
-    <hyperlink ref="I3" r:id="rId2" display="https://www.nvdia.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
@@ -1785,13 +1674,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1807,136 +1696,136 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
         <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="2:3">
       <c r="B4" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="2:3">
       <c r="B5" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="2:3">
       <c r="B6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C7" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="2:3">
       <c r="B8" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="2:3">
       <c r="B9" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="2:3">
       <c r="B10" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C10" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="2:3">
       <c r="B11" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C11" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="2:3">
       <c r="B12" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C12" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="2:3">
       <c r="B13" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C13" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="2:3">
       <c r="B14" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C14" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="3:3">
       <c r="C15" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="3:3">
       <c r="C16" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="3:3">
       <c r="C17" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="3:3">
       <c r="C18" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="3:3">
       <c r="C19" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="3:3">
       <c r="C20" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="3:3">
       <c r="C21" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="3:3">
@@ -1946,72 +1835,72 @@
     </row>
     <row r="23" spans="3:3">
       <c r="C23" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="3:3">
       <c r="C24" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="3:3">
       <c r="C25" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="3:3">
       <c r="C26" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="3:3">
       <c r="C27" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="3:3">
       <c r="C28" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="3:3">
       <c r="C29" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="3:3">
       <c r="C30" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="3:3">
       <c r="C31" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="3:3">
       <c r="C32" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="3:3">
       <c r="C33" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="3:3">
       <c r="C34" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="3:3">
       <c r="C35" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="3:3">
       <c r="C36" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>